<commit_message>
New PO forecast model
</commit_message>
<xml_diff>
--- a/po_analysis_by_asin/B01IEO05NU_po_data.xlsx
+++ b/po_analysis_by_asin/B01IEO05NU_po_data.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B61"/>
+  <dimension ref="A1:B62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -931,6 +931,14 @@
         <v>60</v>
       </c>
     </row>
+    <row r="62">
+      <c r="A62" s="2" t="n">
+        <v>45662.99999999999</v>
+      </c>
+      <c r="B62" t="n">
+        <v>150</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -942,7 +950,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1114,6 +1122,14 @@
         <v>4080</v>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" s="2" t="n">
+        <v>45688.99999999999</v>
+      </c>
+      <c r="B21" t="n">
+        <v>150</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1125,7 +1141,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B69"/>
+  <dimension ref="A1:B70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1150,7 +1166,7 @@
         <v>44934.99999999999</v>
       </c>
       <c r="B2" t="n">
-        <v>140</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3">
@@ -1158,7 +1174,7 @@
         <v>44941.99999999999</v>
       </c>
       <c r="B3" t="n">
-        <v>146</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4">
@@ -1166,7 +1182,7 @@
         <v>44955.99999999999</v>
       </c>
       <c r="B4" t="n">
-        <v>158</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5">
@@ -1174,7 +1190,7 @@
         <v>44962.99999999999</v>
       </c>
       <c r="B5" t="n">
-        <v>164</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6">
@@ -1182,7 +1198,7 @@
         <v>44969.99999999999</v>
       </c>
       <c r="B6" t="n">
-        <v>170</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7">
@@ -1190,7 +1206,7 @@
         <v>44976.99999999999</v>
       </c>
       <c r="B7" t="n">
-        <v>176</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8">
@@ -1198,7 +1214,7 @@
         <v>44983.99999999999</v>
       </c>
       <c r="B8" t="n">
-        <v>182</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9">
@@ -1206,7 +1222,7 @@
         <v>44990.99999999999</v>
       </c>
       <c r="B9" t="n">
-        <v>188</v>
+        <v>201</v>
       </c>
     </row>
     <row r="10">
@@ -1214,7 +1230,7 @@
         <v>44997.99999999999</v>
       </c>
       <c r="B10" t="n">
-        <v>194</v>
+        <v>207</v>
       </c>
     </row>
     <row r="11">
@@ -1222,7 +1238,7 @@
         <v>45004.99999999999</v>
       </c>
       <c r="B11" t="n">
-        <v>200</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12">
@@ -1230,7 +1246,7 @@
         <v>45011.99999999999</v>
       </c>
       <c r="B12" t="n">
-        <v>206</v>
+        <v>217</v>
       </c>
     </row>
     <row r="13">
@@ -1238,7 +1254,7 @@
         <v>45018.99999999999</v>
       </c>
       <c r="B13" t="n">
-        <v>212</v>
+        <v>223</v>
       </c>
     </row>
     <row r="14">
@@ -1246,7 +1262,7 @@
         <v>45025.99999999999</v>
       </c>
       <c r="B14" t="n">
-        <v>218</v>
+        <v>228</v>
       </c>
     </row>
     <row r="15">
@@ -1254,7 +1270,7 @@
         <v>45039.99999999999</v>
       </c>
       <c r="B15" t="n">
-        <v>230</v>
+        <v>239</v>
       </c>
     </row>
     <row r="16">
@@ -1262,7 +1278,7 @@
         <v>45046.99999999999</v>
       </c>
       <c r="B16" t="n">
-        <v>236</v>
+        <v>244</v>
       </c>
     </row>
     <row r="17">
@@ -1270,7 +1286,7 @@
         <v>45053.99999999999</v>
       </c>
       <c r="B17" t="n">
-        <v>242</v>
+        <v>250</v>
       </c>
     </row>
     <row r="18">
@@ -1278,7 +1294,7 @@
         <v>45060.99999999999</v>
       </c>
       <c r="B18" t="n">
-        <v>248</v>
+        <v>255</v>
       </c>
     </row>
     <row r="19">
@@ -1286,7 +1302,7 @@
         <v>45067.99999999999</v>
       </c>
       <c r="B19" t="n">
-        <v>254</v>
+        <v>261</v>
       </c>
     </row>
     <row r="20">
@@ -1294,7 +1310,7 @@
         <v>45088.99999999999</v>
       </c>
       <c r="B20" t="n">
-        <v>272</v>
+        <v>277</v>
       </c>
     </row>
     <row r="21">
@@ -1302,7 +1318,7 @@
         <v>45095.99999999999</v>
       </c>
       <c r="B21" t="n">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
     <row r="22">
@@ -1310,7 +1326,7 @@
         <v>45102.99999999999</v>
       </c>
       <c r="B22" t="n">
-        <v>284</v>
+        <v>288</v>
       </c>
     </row>
     <row r="23">
@@ -1318,7 +1334,7 @@
         <v>45109.99999999999</v>
       </c>
       <c r="B23" t="n">
-        <v>290</v>
+        <v>293</v>
       </c>
     </row>
     <row r="24">
@@ -1326,7 +1342,7 @@
         <v>45123.99999999999</v>
       </c>
       <c r="B24" t="n">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="25">
@@ -1334,7 +1350,7 @@
         <v>45151.99999999999</v>
       </c>
       <c r="B25" t="n">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="26">
@@ -1342,7 +1358,7 @@
         <v>45158.99999999999</v>
       </c>
       <c r="B26" t="n">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="27">
@@ -1350,7 +1366,7 @@
         <v>45165.99999999999</v>
       </c>
       <c r="B27" t="n">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="28">
@@ -1358,7 +1374,7 @@
         <v>45172.99999999999</v>
       </c>
       <c r="B28" t="n">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="29">
@@ -1366,7 +1382,7 @@
         <v>45179.99999999999</v>
       </c>
       <c r="B29" t="n">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="30">
@@ -1374,7 +1390,7 @@
         <v>45186.99999999999</v>
       </c>
       <c r="B30" t="n">
-        <v>357</v>
+        <v>352</v>
       </c>
     </row>
     <row r="31">
@@ -1382,7 +1398,7 @@
         <v>45193.99999999999</v>
       </c>
       <c r="B31" t="n">
-        <v>363</v>
+        <v>358</v>
       </c>
     </row>
     <row r="32">
@@ -1390,7 +1406,7 @@
         <v>45207.99999999999</v>
       </c>
       <c r="B32" t="n">
-        <v>375</v>
+        <v>368</v>
       </c>
     </row>
     <row r="33">
@@ -1398,7 +1414,7 @@
         <v>45214.99999999999</v>
       </c>
       <c r="B33" t="n">
-        <v>381</v>
+        <v>374</v>
       </c>
     </row>
     <row r="34">
@@ -1406,7 +1422,7 @@
         <v>45221.99999999999</v>
       </c>
       <c r="B34" t="n">
-        <v>387</v>
+        <v>379</v>
       </c>
     </row>
     <row r="35">
@@ -1414,7 +1430,7 @@
         <v>45228.99999999999</v>
       </c>
       <c r="B35" t="n">
-        <v>393</v>
+        <v>384</v>
       </c>
     </row>
     <row r="36">
@@ -1422,7 +1438,7 @@
         <v>45333.99999999999</v>
       </c>
       <c r="B36" t="n">
-        <v>484</v>
+        <v>465</v>
       </c>
     </row>
     <row r="37">
@@ -1430,7 +1446,7 @@
         <v>45347.99999999999</v>
       </c>
       <c r="B37" t="n">
-        <v>496</v>
+        <v>476</v>
       </c>
     </row>
     <row r="38">
@@ -1438,7 +1454,7 @@
         <v>45354.99999999999</v>
       </c>
       <c r="B38" t="n">
-        <v>502</v>
+        <v>481</v>
       </c>
     </row>
     <row r="39">
@@ -1446,7 +1462,7 @@
         <v>45361.99999999999</v>
       </c>
       <c r="B39" t="n">
-        <v>508</v>
+        <v>487</v>
       </c>
     </row>
     <row r="40">
@@ -1454,7 +1470,7 @@
         <v>45368.99999999999</v>
       </c>
       <c r="B40" t="n">
-        <v>514</v>
+        <v>492</v>
       </c>
     </row>
     <row r="41">
@@ -1462,7 +1478,7 @@
         <v>45375.99999999999</v>
       </c>
       <c r="B41" t="n">
-        <v>520</v>
+        <v>498</v>
       </c>
     </row>
     <row r="42">
@@ -1470,7 +1486,7 @@
         <v>45382.99999999999</v>
       </c>
       <c r="B42" t="n">
-        <v>526</v>
+        <v>503</v>
       </c>
     </row>
     <row r="43">
@@ -1478,7 +1494,7 @@
         <v>45389.99999999999</v>
       </c>
       <c r="B43" t="n">
-        <v>532</v>
+        <v>508</v>
       </c>
     </row>
     <row r="44">
@@ -1486,7 +1502,7 @@
         <v>45396.99999999999</v>
       </c>
       <c r="B44" t="n">
-        <v>538</v>
+        <v>514</v>
       </c>
     </row>
     <row r="45">
@@ -1494,7 +1510,7 @@
         <v>45403.99999999999</v>
       </c>
       <c r="B45" t="n">
-        <v>544</v>
+        <v>519</v>
       </c>
     </row>
     <row r="46">
@@ -1502,7 +1518,7 @@
         <v>45417.99999999999</v>
       </c>
       <c r="B46" t="n">
-        <v>556</v>
+        <v>530</v>
       </c>
     </row>
     <row r="47">
@@ -1510,7 +1526,7 @@
         <v>45424.99999999999</v>
       </c>
       <c r="B47" t="n">
-        <v>562</v>
+        <v>535</v>
       </c>
     </row>
     <row r="48">
@@ -1518,7 +1534,7 @@
         <v>45431.99999999999</v>
       </c>
       <c r="B48" t="n">
-        <v>568</v>
+        <v>541</v>
       </c>
     </row>
     <row r="49">
@@ -1526,7 +1542,7 @@
         <v>45438.99999999999</v>
       </c>
       <c r="B49" t="n">
-        <v>574</v>
+        <v>546</v>
       </c>
     </row>
     <row r="50">
@@ -1534,7 +1550,7 @@
         <v>45445.99999999999</v>
       </c>
       <c r="B50" t="n">
-        <v>580</v>
+        <v>552</v>
       </c>
     </row>
     <row r="51">
@@ -1542,7 +1558,7 @@
         <v>45459.99999999999</v>
       </c>
       <c r="B51" t="n">
-        <v>592</v>
+        <v>562</v>
       </c>
     </row>
     <row r="52">
@@ -1550,7 +1566,7 @@
         <v>45466.99999999999</v>
       </c>
       <c r="B52" t="n">
-        <v>598</v>
+        <v>568</v>
       </c>
     </row>
     <row r="53">
@@ -1558,7 +1574,7 @@
         <v>45473.99999999999</v>
       </c>
       <c r="B53" t="n">
-        <v>604</v>
+        <v>573</v>
       </c>
     </row>
     <row r="54">
@@ -1566,7 +1582,7 @@
         <v>45480.99999999999</v>
       </c>
       <c r="B54" t="n">
-        <v>610</v>
+        <v>578</v>
       </c>
     </row>
     <row r="55">
@@ -1574,7 +1590,7 @@
         <v>45487.99999999999</v>
       </c>
       <c r="B55" t="n">
-        <v>616</v>
+        <v>584</v>
       </c>
     </row>
     <row r="56">
@@ -1582,7 +1598,7 @@
         <v>45529.99999999999</v>
       </c>
       <c r="B56" t="n">
-        <v>653</v>
+        <v>616</v>
       </c>
     </row>
     <row r="57">
@@ -1590,7 +1606,7 @@
         <v>45536.99999999999</v>
       </c>
       <c r="B57" t="n">
-        <v>659</v>
+        <v>622</v>
       </c>
     </row>
     <row r="58">
@@ -1598,7 +1614,7 @@
         <v>45578.99999999999</v>
       </c>
       <c r="B58" t="n">
-        <v>695</v>
+        <v>654</v>
       </c>
     </row>
     <row r="59">
@@ -1606,7 +1622,7 @@
         <v>45599.99999999999</v>
       </c>
       <c r="B59" t="n">
-        <v>713</v>
+        <v>670</v>
       </c>
     </row>
     <row r="60">
@@ -1614,7 +1630,7 @@
         <v>45606.99999999999</v>
       </c>
       <c r="B60" t="n">
-        <v>719</v>
+        <v>675</v>
       </c>
     </row>
     <row r="61">
@@ -1622,71 +1638,79 @@
         <v>45613.99999999999</v>
       </c>
       <c r="B61" t="n">
-        <v>725</v>
+        <v>681</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="2" t="n">
-        <v>45620.99999999999</v>
+        <v>45662.99999999999</v>
       </c>
       <c r="B62" t="n">
-        <v>731</v>
+        <v>719</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="2" t="n">
-        <v>45627.99999999999</v>
+        <v>45669.99999999999</v>
       </c>
       <c r="B63" t="n">
-        <v>737</v>
+        <v>724</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="2" t="n">
-        <v>45634.99999999999</v>
+        <v>45676.99999999999</v>
       </c>
       <c r="B64" t="n">
-        <v>743</v>
+        <v>729</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="2" t="n">
-        <v>45641.99999999999</v>
+        <v>45683.99999999999</v>
       </c>
       <c r="B65" t="n">
-        <v>749</v>
+        <v>735</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="2" t="n">
-        <v>45648.99999999999</v>
+        <v>45690.99999999999</v>
       </c>
       <c r="B66" t="n">
-        <v>755</v>
+        <v>740</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="2" t="n">
-        <v>45655.99999999999</v>
+        <v>45697.99999999999</v>
       </c>
       <c r="B67" t="n">
-        <v>761</v>
+        <v>746</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="2" t="n">
-        <v>45662.99999999999</v>
+        <v>45704.99999999999</v>
       </c>
       <c r="B68" t="n">
-        <v>767</v>
+        <v>751</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="2" t="n">
-        <v>45669.99999999999</v>
+        <v>45711.99999999999</v>
       </c>
       <c r="B69" t="n">
-        <v>773</v>
+        <v>756</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="2" t="n">
+        <v>45718.99999999999</v>
+      </c>
+      <c r="B70" t="n">
+        <v>762</v>
       </c>
     </row>
   </sheetData>

</xml_diff>